<commit_message>
Começo da utilização de pageFactory e excel com dados
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
+++ b/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoTDD\src\br\com\rsinet\HUB_TDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13B57425-FA76-43DA-AEF3-62E1451F5168}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73241B31-B473-4721-A591-1BABE227C419}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,9 +30,68 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+  <si>
+    <t>userName</t>
+  </si>
+  <si>
+    <t>userPass</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>FristName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>AbdielCordeiro</t>
+  </si>
+  <si>
+    <t>Trocar@123</t>
+  </si>
+  <si>
+    <t>abdiel.cordeiro@rsinet.com.br</t>
+  </si>
+  <si>
+    <t>Abdiel</t>
+  </si>
+  <si>
+    <t>Cordeiro</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>City</t>
+  </si>
+  <si>
+    <t>Osasco</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>Rua Antonio Bertoldo de Oliveira</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>São Paulo</t>
+  </si>
+  <si>
+    <t>CEP</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -40,13 +99,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -58,13 +145,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -377,14 +479,104 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="13.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.88671875" style="2"/>
+    <col min="8" max="8" width="28.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="4">
+        <v>11987672784</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="4">
+        <v>6290060</v>
+      </c>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{46AC47A1-1F89-45AF-8C7B-F4A195208066}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{85BD8E5A-7C04-41EF-BADE-536F55EA589D}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Teste de falha com PageFactory e Massa de dados
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
+++ b/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoTDD\src\br\com\rsinet\HUB_TDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73241B31-B473-4721-A591-1BABE227C419}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F62BB84-C37C-4A98-8155-19B5D5F1BEB6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>userName</t>
   </si>
@@ -48,9 +48,6 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>AbdielCordeiro</t>
-  </si>
-  <si>
     <t>Trocar@123</t>
   </si>
   <si>
@@ -85,6 +82,15 @@
   </si>
   <si>
     <t>CEP</t>
+  </si>
+  <si>
+    <t>06290-060</t>
+  </si>
+  <si>
+    <t>1198767-2784</t>
+  </si>
+  <si>
+    <t>AbdielCCCCordeiro</t>
   </si>
 </sst>
 </file>
@@ -110,7 +116,7 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -145,11 +151,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -161,12 +166,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -479,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -495,7 +500,9 @@
     <col min="6" max="6" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8.88671875" style="2"/>
     <col min="8" max="8" width="28.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="2"/>
+    <col min="9" max="10" width="8.88671875" style="2"/>
+    <col min="11" max="11" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
@@ -515,19 +522,19 @@
         <v>4</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>11</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
@@ -536,40 +543,43 @@
       <c r="O1" s="1"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" s="4">
-        <v>11987672784</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="4">
-        <v>6290060</v>
-      </c>
-      <c r="K2" s="4"/>
+      <c r="F2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="5"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Busca produto sucesso pela lupa em pagefactory e parte em massa
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
+++ b/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoTDD\src\br\com\rsinet\HUB_TDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F62BB84-C37C-4A98-8155-19B5D5F1BEB6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA59AFF-BB9A-4D9A-9534-F90B31B9AEE6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
+    <workbookView xWindow="4044" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
+    <sheet name="Pesquisa" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>userName</t>
   </si>
@@ -91,6 +92,15 @@
   </si>
   <si>
     <t>AbdielCCCCordeiro</t>
+  </si>
+  <si>
+    <t>Produto</t>
+  </si>
+  <si>
+    <t>Mice</t>
+  </si>
+  <si>
+    <t>nomeProduto</t>
   </si>
 </sst>
 </file>
@@ -154,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -170,6 +180,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,8 +497,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -589,4 +600,42 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9334BD-5787-4860-8F04-DE32560FFDB3}">
+  <dimension ref="A1:H12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="4"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H12" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Busca pela lupa com erro com page factory e massa de dados
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
+++ b/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoTDD\src\br\com\rsinet\HUB_TDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA59AFF-BB9A-4D9A-9534-F90B31B9AEE6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528D5CB4-A6BA-45E2-B3F2-A2E39095145B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4044" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
@@ -97,10 +97,10 @@
     <t>Produto</t>
   </si>
   <si>
-    <t>Mice</t>
-  </si>
-  <si>
     <t>nomeProduto</t>
+  </si>
+  <si>
+    <t>Banana</t>
   </si>
 </sst>
 </file>
@@ -164,7 +164,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -181,6 +181,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -607,7 +610,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -622,12 +625,12 @@
         <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>21</v>
+      <c r="A2" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="B2" s="4"/>
     </row>

</xml_diff>

<commit_message>
Adicionando TestNG em todos os casos de teste
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
+++ b/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoTDD\src\br\com\rsinet\HUB_TDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{528D5CB4-A6BA-45E2-B3F2-A2E39095145B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B80156C-3C8E-4A57-BF22-9D95BBC64FA3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4044" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
@@ -100,7 +100,7 @@
     <t>nomeProduto</t>
   </si>
   <si>
-    <t>Banana</t>
+    <t>Mandioca</t>
   </si>
 </sst>
 </file>
@@ -610,7 +610,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Correção de alguns erros e assert no caso de teste sucesso
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
+++ b/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoTDD\src\br\com\rsinet\HUB_TDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B80156C-3C8E-4A57-BF22-9D95BBC64FA3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559BC552-B406-4BAA-BADB-C2392A37AE43}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4044" yWindow="3396" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -91,9 +91,6 @@
     <t>1198767-2784</t>
   </si>
   <si>
-    <t>AbdielCCCCordeiro</t>
-  </si>
-  <si>
     <t>Produto</t>
   </si>
   <si>
@@ -101,6 +98,9 @@
   </si>
   <si>
     <t>Mandioca</t>
+  </si>
+  <si>
+    <t>AbdielCrdeiRO</t>
   </si>
 </sst>
 </file>
@@ -500,8 +500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -558,7 +558,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>5</v>
@@ -609,7 +609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9334BD-5787-4860-8F04-DE32560FFDB3}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -622,15 +622,15 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B2" s="4"/>
     </row>

</xml_diff>

<commit_message>
Tela de cadastrar refatorada com nossos pedidos de separação dos metodos
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
+++ b/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoTDD\src\br\com\rsinet\HUB_TDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{559BC552-B406-4BAA-BADB-C2392A37AE43}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A863567-265A-46F7-8DE5-848DF245E56F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>userName</t>
   </si>
@@ -97,10 +97,22 @@
     <t>nomeProduto</t>
   </si>
   <si>
-    <t>Mandioca</t>
-  </si>
-  <si>
-    <t>AbdielCrdeiRO</t>
+    <t>Bose SoundLink Wireless Speaker</t>
+  </si>
+  <si>
+    <t>Speakers</t>
+  </si>
+  <si>
+    <t>HP USB 3 Button Optical Mouse</t>
+  </si>
+  <si>
+    <t>Pais</t>
+  </si>
+  <si>
+    <t>Brazil</t>
+  </si>
+  <si>
+    <t>abdielCordeiro</t>
   </si>
 </sst>
 </file>
@@ -550,7 +562,9 @@
       <c r="J1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="K1" s="3"/>
+      <c r="K1" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
@@ -558,7 +572,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>5</v>
@@ -587,13 +601,16 @@
       <c r="J2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="5"/>
+      <c r="K2" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
+      <c r="K3" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -607,20 +624,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9334BD-5787-4860-8F04-DE32560FFDB3}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="12.77734375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
@@ -628,14 +645,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="6"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H12" s="7"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I15" s="2" t="s">
+        <v>23</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Commit final, todas as cases modificação com os padrões Factory
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
+++ b/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoTDD\src\br\com\rsinet\HUB_TDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A863567-265A-46F7-8DE5-848DF245E56F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E9CD00-1795-4B0A-898B-DBB07E7CF393}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
   <si>
     <t>userName</t>
   </si>
@@ -97,9 +97,6 @@
     <t>nomeProduto</t>
   </si>
   <si>
-    <t>Bose SoundLink Wireless Speaker</t>
-  </si>
-  <si>
     <t>Speakers</t>
   </si>
   <si>
@@ -112,7 +109,37 @@
     <t>Brazil</t>
   </si>
   <si>
-    <t>abdielCordeiro</t>
+    <t>Bose Soundlink Bluetooth Speaker III</t>
+  </si>
+  <si>
+    <t>Mice</t>
+  </si>
+  <si>
+    <t>Descricao</t>
+  </si>
+  <si>
+    <t>Sucesso</t>
+  </si>
+  <si>
+    <t>Falha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bose Soundlink Bluetooth Speaker </t>
+  </si>
+  <si>
+    <t>Laptops</t>
+  </si>
+  <si>
+    <t>HP Chromebook 14 G1(ENERGY STAR)</t>
+  </si>
+  <si>
+    <t>Banana</t>
+  </si>
+  <si>
+    <t>Mochila</t>
+  </si>
+  <si>
+    <t>lucasViado</t>
   </si>
 </sst>
 </file>
@@ -518,7 +545,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
@@ -563,7 +590,7 @@
         <v>16</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -572,7 +599,7 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>5</v>
@@ -602,7 +629,7 @@
         <v>17</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
@@ -624,45 +651,95 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9334BD-5787-4860-8F04-DE32560FFDB3}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="30.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C1" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="6"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C4" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="F9" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="H12" s="7"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="I15" s="2" t="s">
-        <v>23</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Ajustes na massa de dados e alguns ajustes
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
+++ b/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoTDD\src\br\com\rsinet\HUB_TDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD83952-37E0-4BB7-B620-8F4F90083EF7}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0787311-8E3D-4777-B3A0-D849427F6112}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
@@ -32,19 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
-  <si>
-    <t>userName</t>
-  </si>
-  <si>
-    <t>userPass</t>
-  </si>
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>FristName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="38">
   <si>
     <t>LastName</t>
   </si>
@@ -61,18 +49,12 @@
     <t>Cordeiro</t>
   </si>
   <si>
-    <t>phoneNumber</t>
-  </si>
-  <si>
     <t>City</t>
   </si>
   <si>
     <t>Osasco</t>
   </si>
   <si>
-    <t>address</t>
-  </si>
-  <si>
     <t>Rua Antonio Bertoldo de Oliveira</t>
   </si>
   <si>
@@ -82,9 +64,6 @@
     <t>São Paulo</t>
   </si>
   <si>
-    <t>CEP</t>
-  </si>
-  <si>
     <t>06290-060</t>
   </si>
   <si>
@@ -103,9 +82,6 @@
     <t>HP USB 3 Button Optical Mouse</t>
   </si>
   <si>
-    <t>Pais</t>
-  </si>
-  <si>
     <t>Brazil</t>
   </si>
   <si>
@@ -124,9 +100,6 @@
     <t>Falha</t>
   </si>
   <si>
-    <t xml:space="preserve">Bose Soundlink Bluetooth Speaker </t>
-  </si>
-  <si>
     <t>Laptops</t>
   </si>
   <si>
@@ -139,7 +112,40 @@
     <t>Mochila</t>
   </si>
   <si>
-    <t>lucasViado</t>
+    <t>lucasViadoadasdda</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>PostalCode</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>UserNameFalha</t>
+  </si>
+  <si>
+    <t>UserPass</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Quantidade</t>
+  </si>
+  <si>
+    <t>abdielCordeiro2</t>
   </si>
 </sst>
 </file>
@@ -203,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -221,6 +227,9 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -537,112 +546,127 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.88671875" style="2"/>
-    <col min="8" max="8" width="28.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.88671875" style="2"/>
-    <col min="11" max="11" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="16.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" style="2"/>
+    <col min="9" max="9" width="28.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.88671875" style="2"/>
+    <col min="11" max="11" width="10.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>9</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="L1" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="M1" s="3"/>
       <c r="N1" s="3"/>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O1" s="3"/>
+      <c r="P1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>11</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="I2" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="K2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
-      <c r="K3" s="7"/>
+      <c r="B3" s="6"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="D5" s="6"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K7" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{46AC47A1-1F89-45AF-8C7B-F4A195208066}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{85BD8E5A-7C04-41EF-BADE-536F55EA589D}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{46AC47A1-1F89-45AF-8C7B-F4A195208066}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{85BD8E5A-7C04-41EF-BADE-536F55EA589D}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
@@ -651,95 +675,92 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9334BD-5787-4860-8F04-DE32560FFDB3}">
-  <dimension ref="A1:H12"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2"/>
     <col min="2" max="2" width="36.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="2"/>
+    <col min="3" max="4" width="8.88671875" style="2"/>
+    <col min="5" max="5" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>27</v>
+      <c r="E1" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="E2" s="9">
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F9" s="6"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H12" s="7"/>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="H11" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Report com print no relatorio
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
+++ b/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoTDD\src\br\com\rsinet\HUB_TDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23D5930-EEDE-4734-AB36-C6A94AA5AE52}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D72CE97-BBE4-470F-B4B2-C4579CE92A01}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
     <t>Quantidade</t>
   </si>
   <si>
-    <t>abdielCordeiro2</t>
+    <t>abdielCordeir16</t>
   </si>
 </sst>
 </file>
@@ -549,7 +549,7 @@
   <dimension ref="A1:P7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Retirada de um System.out.println()
</commit_message>
<xml_diff>
--- a/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
+++ b/src/br/com/rsinet/HUB_TDD/testData/BancoDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoTDD\src\br\com\rsinet\HUB_TDD\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D72CE97-BBE4-470F-B4B2-C4579CE92A01}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB1AC6A-E2C0-46D1-B598-02606C48F8E9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -145,7 +145,7 @@
     <t>Quantidade</t>
   </si>
   <si>
-    <t>abdielCordeir16</t>
+    <t>2abdielCordeir1</t>
   </si>
 </sst>
 </file>

</xml_diff>